<commit_message>
Signed-off-by: Umair Nasir Ahmad <umairnasirahmad@gmail.com>
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\noteballs\vue-composition-api-noteballs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A7E9B85-D969-48D9-928F-E1C7B2143BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8332B1BD-9516-4BCF-860C-27B52B5C53F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8B1A7BBB-FB8B-4AC2-A08A-5E319C73BCD8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>test sheet 1</t>
+    <t>test sheet 1 changed</t>
   </si>
 </sst>
 </file>
@@ -412,9 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AED6BDD-EE33-402E-8DCA-E943D15F80B6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>